<commit_message>
amélioration de la bdd
</commit_message>
<xml_diff>
--- a/uploads/L3GL.xlsx
+++ b/uploads/L3GL.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t xml:space="preserve">NOMETUDIANT</t>
+    <t xml:space="preserve">NOM ETUDIANT</t>
   </si>
   <si>
     <t xml:space="preserve">POO</t>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">LANGAGE SQL</t>
   </si>
   <si>
-    <t xml:space="preserve">DEVELOPPEMENT WEB</t>
+    <t xml:space="preserve">DEVELOPEMENT WEB</t>
   </si>
   <si>
     <t xml:space="preserve">PHN</t>
@@ -275,12 +275,12 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>